<commit_message>
debugged figure gdp 70-18
</commit_message>
<xml_diff>
--- a/data/economy/deflator implicito do pib ipea.xlsx
+++ b/data/economy/deflator implicito do pib ipea.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/600ce01881951ac9/Acadêmico/academic apps/br metro economic/data/economy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EAF2F42B-BCD1-42B3-B992-FEBC62C6C63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:40009_{EAF2F42B-BCD1-42B3-B992-FEBC62C6C63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9284EC84-17B5-43EA-8D1B-FAE304C742F9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="deflator implicito do pib ipea" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,10 +42,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -545,11 +556,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -905,11 +916,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,7 +930,8 @@
     <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1208,6 +1220,9 @@
       <c r="B34">
         <v>30.825383380000002</v>
       </c>
+      <c r="L34">
+        <v>374518969.19999999</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -1232,6 +1247,12 @@
       <c r="B37">
         <v>40.711402790000001</v>
       </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>374518969.19999999</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -1240,8 +1261,12 @@
       <c r="B38">
         <v>43.469304809999997</v>
       </c>
+      <c r="K38" s="2">
+        <v>283840192</v>
+      </c>
       <c r="L38" s="4">
-        <v>374518969</v>
+        <f>K38*B42/B38</f>
+        <v>382380004.55660164</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -1293,12 +1318,12 @@
         <v>27132250968.041759</v>
       </c>
       <c r="F42">
-        <f>B42/B50</f>
-        <v>0.58560392220000002</v>
+        <f>B42/B49</f>
+        <v>0.61191823547125335</v>
       </c>
       <c r="G42">
         <f>C42/F42</f>
-        <v>27132250968.041756</v>
+        <v>25965483072.691368</v>
       </c>
       <c r="H42">
         <v>1.707638835893029</v>
@@ -1314,6 +1339,10 @@
       </c>
       <c r="B43">
         <v>63.431792450000003</v>
+      </c>
+      <c r="H43">
+        <f>G42/C42</f>
+        <v>1.6342052614756206</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>